<commit_message>
working notifying human flow
</commit_message>
<xml_diff>
--- a/capstone_project_db_management/database.xlsx
+++ b/capstone_project_db_management/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>followed_up</t>
+          <t>notified_human</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>followed_up</t>
+          <t>notified_human</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>followed_up</t>
+          <t>notified_human</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>followed_up</t>
+          <t>notified_human</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>followed_up</t>
+          <t>notified_human</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1585,6 +1585,1106 @@
         </is>
       </c>
       <c r="K21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CUST021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Andrew Martinez</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>andrew.m@tech.start</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+91-9876543230</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>65000</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CUST022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Julia Roberts</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>julia.r@creative.co</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+91-9876543231</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Graphic Design</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>24000</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CUST023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Chris Evans</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>chris.e@enterprise.io</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+91-9876543232</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>38000</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CUST024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Emma Watson</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>emma.w@digital.net</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+91-9876543233</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Content Strategy</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CUST025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Robert Lee</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>robert.l@cloud.tech</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+91-9876543234</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Blockchain</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>72000</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CUST021</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Andrew Martinez</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>andrew.m@tech.start</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>+91-9876543230</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>65000</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CUST022</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Julia Roberts</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>julia.r@creative.co</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>+91-9876543231</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Graphic Design</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>24000</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CUST023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Chris Evans</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>chris.e@enterprise.io</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>+91-9876543232</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>38000</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CUST024</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Emma Watson</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>emma.w@digital.net</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>+91-9876543233</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Content Strategy</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CUST025</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Robert Lee</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>robert.l@cloud.tech</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>+91-9876543234</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Blockchain</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>72000</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CUST021</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Andrew Martinez</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>andrew.m@tech.start</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>+91-9876543230</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>65000</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CUST022</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Julia Roberts</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>julia.r@creative.co</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>+91-9876543231</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Graphic Design</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>24000</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CUST023</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Chris Evans</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>chris.e@enterprise.io</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>+91-9876543232</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>38000</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CUST024</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Emma Watson</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>emma.w@digital.net</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>+91-9876543233</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Content Strategy</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CUST025</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Robert Lee</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>robert.l@cloud.tech</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>+91-9876543234</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Blockchain</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>72000</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CUST021</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Andrew Martinez</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>andrew.m@tech.start</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>+91-9876543230</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>65000</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CUST022</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Julia Roberts</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>julia.r@creative.co</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>+91-9876543231</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Graphic Design</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>24000</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CUST023</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Chris Evans</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>chris.e@enterprise.io</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>+91-9876543232</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>38000</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CUST024</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Emma Watson</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>emma.w@digital.net</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>+91-9876543233</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Content Strategy</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CUST025</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Robert Lee</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>robert.l@cloud.tech</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>+91-9876543234</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Blockchain</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>72000</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>unprocessed</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>yes</t>
         </is>

</xml_diff>